<commit_message>
client int_addr to inet_pton and bug fixes
added default or custom settings to client
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FICOR\Documents\SO-TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB0068D7-79AC-4B0C-841D-A22DB42334DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A25DDDF-A4FD-4D0B-9298-D4E067396997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{48C1C086-06C7-45D6-831B-E997FC3942EF}"/>
   </bookViews>
@@ -17,11 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$ALL$1</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$ALK$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$ALL$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$1:$ALL$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$AKZ$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$1:$ALL$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$ALL$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -107,7 +103,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1064,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BEE45C-1BD0-428E-924A-938B6C0DD9B4}">
-  <dimension ref="A1:ALL1"/>
+  <dimension ref="A1:BXF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AKU1" workbookViewId="0">
-      <selection activeCell="ALF8" sqref="ALF8"/>
+    <sheetView tabSelected="1" topLeftCell="AKV1" workbookViewId="0">
+      <selection activeCell="ALJ10" sqref="ALJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,7 +1075,7 @@
     <col min="1000" max="1000" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1000" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1982" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>-0.63800999999999997</v>
       </c>
@@ -4079,6 +4075,3024 @@
       </c>
       <c r="ALL1" s="1">
         <v>-0.20330899999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1982" x14ac:dyDescent="0.35">
+      <c r="AKU2">
+        <v>0.84029900000000002</v>
+      </c>
+      <c r="AKV2">
+        <v>7.6356999999999994E-2</v>
+      </c>
+      <c r="AKW2">
+        <v>-1.391516</v>
+      </c>
+      <c r="AKX2">
+        <v>0.59098499999999998</v>
+      </c>
+      <c r="AKY2">
+        <v>-4.5075999999999998E-2</v>
+      </c>
+      <c r="AKZ2">
+        <v>-0.17483399999999999</v>
+      </c>
+      <c r="ALA2">
+        <v>-0.65451800000000004</v>
+      </c>
+      <c r="ALB2">
+        <v>-0.80928900000000004</v>
+      </c>
+      <c r="ALC2">
+        <v>1.613243</v>
+      </c>
+      <c r="ALD2">
+        <v>2.49831</v>
+      </c>
+      <c r="ALE2">
+        <v>4.6891000000000002E-2</v>
+      </c>
+      <c r="ALF2">
+        <v>1.7230559999999999</v>
+      </c>
+      <c r="ALG2">
+        <v>0.34278500000000001</v>
+      </c>
+      <c r="ALH2">
+        <v>1.5489299999999999</v>
+      </c>
+      <c r="ALI2">
+        <v>-0.19156200000000001</v>
+      </c>
+      <c r="ALJ2">
+        <v>-0.58311000000000002</v>
+      </c>
+      <c r="ALK2">
+        <v>-3.7203E-2</v>
+      </c>
+      <c r="ALL2">
+        <v>1.311933</v>
+      </c>
+      <c r="ALM2">
+        <v>-1.6081240000000001</v>
+      </c>
+      <c r="ALN2">
+        <v>0.325293</v>
+      </c>
+      <c r="ALO2">
+        <v>-1.4753210000000001</v>
+      </c>
+      <c r="ALP2">
+        <v>-0.46074100000000001</v>
+      </c>
+      <c r="ALQ2">
+        <v>-0.490508</v>
+      </c>
+      <c r="ALR2">
+        <v>1.7845519999999999</v>
+      </c>
+      <c r="ALS2">
+        <v>1.071429</v>
+      </c>
+      <c r="ALT2">
+        <v>0.48455100000000001</v>
+      </c>
+      <c r="ALU2">
+        <v>0.38283699999999998</v>
+      </c>
+      <c r="ALV2">
+        <v>-0.17103499999999999</v>
+      </c>
+      <c r="ALW2">
+        <v>0.119256</v>
+      </c>
+      <c r="ALX2">
+        <v>0.83437600000000001</v>
+      </c>
+      <c r="ALY2">
+        <v>-0.48018300000000003</v>
+      </c>
+      <c r="ALZ2">
+        <v>-0.979603</v>
+      </c>
+      <c r="AMA2">
+        <v>1.9234789999999999</v>
+      </c>
+      <c r="AMB2">
+        <v>-0.61022600000000005</v>
+      </c>
+      <c r="AMC2">
+        <v>0.30579000000000001</v>
+      </c>
+      <c r="AMD2">
+        <v>0.323986</v>
+      </c>
+      <c r="AME2">
+        <v>-0.52652399999999999</v>
+      </c>
+      <c r="AMF2">
+        <v>-1.232329</v>
+      </c>
+      <c r="AMG2">
+        <v>-0.14262</v>
+      </c>
+      <c r="AMH2">
+        <v>-3.9802999999999998E-2</v>
+      </c>
+      <c r="AMI2">
+        <v>0.49558200000000002</v>
+      </c>
+      <c r="AMJ2">
+        <v>0.58511299999999999</v>
+      </c>
+      <c r="AMK2">
+        <v>0.31587300000000001</v>
+      </c>
+      <c r="AML2">
+        <v>0.414051</v>
+      </c>
+      <c r="AMM2">
+        <v>-2.4767000000000001</v>
+      </c>
+      <c r="AMN2">
+        <v>0.26413599999999998</v>
+      </c>
+      <c r="AMO2">
+        <v>-0.308006</v>
+      </c>
+      <c r="AMP2">
+        <v>1.6990190000000001</v>
+      </c>
+      <c r="AMQ2">
+        <v>-0.96375200000000005</v>
+      </c>
+      <c r="AMR2">
+        <v>0.38734400000000002</v>
+      </c>
+      <c r="AMS2">
+        <v>0.21148</v>
+      </c>
+      <c r="AMT2">
+        <v>-0.76962299999999995</v>
+      </c>
+      <c r="AMU2">
+        <v>0.72271300000000005</v>
+      </c>
+      <c r="AMV2">
+        <v>1.6885349999999999</v>
+      </c>
+      <c r="AMW2">
+        <v>2.1309520000000002</v>
+      </c>
+      <c r="AMX2">
+        <v>-1.640012</v>
+      </c>
+      <c r="AMY2">
+        <v>-0.17230799999999999</v>
+      </c>
+      <c r="AMZ2">
+        <v>-0.108135</v>
+      </c>
+      <c r="ANA2">
+        <v>-1.4730110000000001</v>
+      </c>
+      <c r="ANB2">
+        <v>-0.15312899999999999</v>
+      </c>
+      <c r="ANC2">
+        <v>-2.16988</v>
+      </c>
+      <c r="AND2">
+        <v>2.1110989999999998</v>
+      </c>
+      <c r="ANE2">
+        <v>-0.28556700000000002</v>
+      </c>
+      <c r="ANF2">
+        <v>0.16564999999999999</v>
+      </c>
+      <c r="ANG2">
+        <v>-3.6219000000000001E-2</v>
+      </c>
+      <c r="ANH2">
+        <v>0.18246100000000001</v>
+      </c>
+      <c r="ANI2">
+        <v>-2.1687029999999998</v>
+      </c>
+      <c r="ANJ2">
+        <v>-0.23092399999999999</v>
+      </c>
+      <c r="ANK2">
+        <v>-0.54250399999999999</v>
+      </c>
+      <c r="ANL2">
+        <v>-1.4902200000000001</v>
+      </c>
+      <c r="ANM2">
+        <v>-0.89128600000000002</v>
+      </c>
+      <c r="ANN2">
+        <v>-0.42616199999999999</v>
+      </c>
+      <c r="ANO2">
+        <v>-0.55372399999999999</v>
+      </c>
+      <c r="ANP2">
+        <v>1.782653</v>
+      </c>
+      <c r="ANQ2">
+        <v>1.0822860000000001</v>
+      </c>
+      <c r="ANR2">
+        <v>-0.18165500000000001</v>
+      </c>
+      <c r="ANS2">
+        <v>-1.2517100000000001</v>
+      </c>
+      <c r="ANT2">
+        <v>0.43290499999999998</v>
+      </c>
+      <c r="ANU2">
+        <v>0.206844</v>
+      </c>
+      <c r="ANV2">
+        <v>-0.14813299999999999</v>
+      </c>
+      <c r="ANW2">
+        <v>-0.310282</v>
+      </c>
+      <c r="ANX2">
+        <v>-0.94345000000000001</v>
+      </c>
+      <c r="ANY2">
+        <v>0.63761699999999999</v>
+      </c>
+      <c r="ANZ2">
+        <v>0.32673400000000002</v>
+      </c>
+      <c r="AOA2">
+        <v>0.58591599999999999</v>
+      </c>
+      <c r="AOB2">
+        <v>-0.74378900000000003</v>
+      </c>
+      <c r="AOC2">
+        <v>-0.93900399999999995</v>
+      </c>
+      <c r="AOD2">
+        <v>-0.57594599999999996</v>
+      </c>
+      <c r="AOE2">
+        <v>2.2234090000000002</v>
+      </c>
+      <c r="AOF2">
+        <v>-4.5233000000000002E-2</v>
+      </c>
+      <c r="AOG2">
+        <v>0.18146499999999999</v>
+      </c>
+      <c r="AOH2">
+        <v>0.226551</v>
+      </c>
+      <c r="AOI2">
+        <v>0.18817200000000001</v>
+      </c>
+      <c r="AOJ2">
+        <v>1.2880119999999999</v>
+      </c>
+      <c r="AOK2">
+        <v>4.5504999999999997E-2</v>
+      </c>
+      <c r="AOL2">
+        <v>-0.80343100000000001</v>
+      </c>
+      <c r="AOM2">
+        <v>-0.368315</v>
+      </c>
+      <c r="AON2">
+        <v>1.958134</v>
+      </c>
+      <c r="AOO2">
+        <v>1.2080789999999999</v>
+      </c>
+      <c r="AOP2">
+        <v>2.5679979999999998</v>
+      </c>
+      <c r="AOQ2">
+        <v>-2.058586</v>
+      </c>
+      <c r="AOR2">
+        <v>-0.754104</v>
+      </c>
+      <c r="AOS2">
+        <v>0.458762</v>
+      </c>
+      <c r="AOT2">
+        <v>0.67721500000000001</v>
+      </c>
+      <c r="AOU2">
+        <v>-1.3918470000000001</v>
+      </c>
+      <c r="AOV2">
+        <v>1.0228459999999999</v>
+      </c>
+      <c r="AOW2">
+        <v>1.3357490000000001</v>
+      </c>
+      <c r="AOX2">
+        <v>-1.072163</v>
+      </c>
+      <c r="AOY2">
+        <v>-3.1893999999999999E-2</v>
+      </c>
+      <c r="AOZ2">
+        <v>-0.19376099999999999</v>
+      </c>
+      <c r="APA2">
+        <v>-0.397233</v>
+      </c>
+      <c r="APB2">
+        <v>-1.521803</v>
+      </c>
+      <c r="APC2">
+        <v>0.24093700000000001</v>
+      </c>
+      <c r="APD2">
+        <v>0.86438899999999996</v>
+      </c>
+      <c r="APE2">
+        <v>-2.112689</v>
+      </c>
+      <c r="APF2">
+        <v>0.36887399999999998</v>
+      </c>
+      <c r="APG2">
+        <v>-0.15786800000000001</v>
+      </c>
+      <c r="APH2">
+        <v>-4.4860999999999998E-2</v>
+      </c>
+      <c r="API2">
+        <v>0.92127999999999999</v>
+      </c>
+      <c r="APJ2">
+        <v>-0.31246200000000002</v>
+      </c>
+      <c r="APK2">
+        <v>1.022745</v>
+      </c>
+      <c r="APL2">
+        <v>0.49875199999999997</v>
+      </c>
+      <c r="APM2">
+        <v>0.33957900000000002</v>
+      </c>
+      <c r="APN2">
+        <v>-0.75192700000000001</v>
+      </c>
+      <c r="APO2">
+        <v>0.40312199999999998</v>
+      </c>
+      <c r="APP2">
+        <v>-1.124514</v>
+      </c>
+      <c r="APQ2">
+        <v>-1.2874060000000001</v>
+      </c>
+      <c r="APR2">
+        <v>0.13875899999999999</v>
+      </c>
+      <c r="APS2">
+        <v>-0.75357799999999997</v>
+      </c>
+      <c r="APT2">
+        <v>0.29902499999999999</v>
+      </c>
+      <c r="APU2">
+        <v>6.803E-3</v>
+      </c>
+      <c r="APV2">
+        <v>0.16019900000000001</v>
+      </c>
+      <c r="APW2">
+        <v>-4.9549999999999997E-2</v>
+      </c>
+      <c r="APX2">
+        <v>-1.35592</v>
+      </c>
+      <c r="APY2">
+        <v>0.59346200000000005</v>
+      </c>
+      <c r="APZ2">
+        <v>1.2937799999999999</v>
+      </c>
+      <c r="AQA2">
+        <v>0.72046600000000005</v>
+      </c>
+      <c r="AQB2">
+        <v>-1.681349</v>
+      </c>
+      <c r="AQC2">
+        <v>-1.950734</v>
+      </c>
+      <c r="AQD2">
+        <v>1.554405</v>
+      </c>
+      <c r="AQE2">
+        <v>-0.54679</v>
+      </c>
+      <c r="AQF2">
+        <v>1.2673509999999999</v>
+      </c>
+      <c r="AQG2">
+        <v>-1.45488</v>
+      </c>
+      <c r="AQH2">
+        <v>2.2001870000000001</v>
+      </c>
+      <c r="AQI2">
+        <v>0.48415399999999997</v>
+      </c>
+      <c r="AQJ2">
+        <v>0.46062199999999998</v>
+      </c>
+      <c r="AQK2">
+        <v>2.2624999999999999E-2</v>
+      </c>
+      <c r="AQL2">
+        <v>-0.64242200000000005</v>
+      </c>
+      <c r="AQM2">
+        <v>-0.96181399999999995</v>
+      </c>
+      <c r="AQN2">
+        <v>1.1489780000000001</v>
+      </c>
+      <c r="AQO2">
+        <v>-1.4874769999999999</v>
+      </c>
+      <c r="AQP2">
+        <v>1.6292679999999999</v>
+      </c>
+      <c r="AQQ2">
+        <v>-9.6118999999999996E-2</v>
+      </c>
+      <c r="AQR2">
+        <v>-0.72176899999999999</v>
+      </c>
+      <c r="AQS2">
+        <v>0.69503300000000001</v>
+      </c>
+      <c r="AQT2">
+        <v>-0.86969300000000005</v>
+      </c>
+      <c r="AQU2">
+        <v>0.94767900000000005</v>
+      </c>
+      <c r="AQV2">
+        <v>0.54952900000000005</v>
+      </c>
+      <c r="AQW2">
+        <v>-1.319928</v>
+      </c>
+      <c r="AQX2">
+        <v>-0.13100200000000001</v>
+      </c>
+      <c r="AQY2">
+        <v>-1.196963</v>
+      </c>
+      <c r="AQZ2">
+        <v>1.0738190000000001</v>
+      </c>
+      <c r="ARA2">
+        <v>0.93919699999999995</v>
+      </c>
+      <c r="ARB2">
+        <v>0.15353600000000001</v>
+      </c>
+      <c r="ARC2">
+        <v>0.89585000000000004</v>
+      </c>
+      <c r="ARD2">
+        <v>0.133932</v>
+      </c>
+      <c r="ARE2">
+        <v>0.428226</v>
+      </c>
+      <c r="ARF2">
+        <v>0.59042399999999995</v>
+      </c>
+      <c r="ARG2">
+        <v>-1.248702</v>
+      </c>
+      <c r="ARH2">
+        <v>0.10818999999999999</v>
+      </c>
+      <c r="ARI2">
+        <v>0.52413699999999996</v>
+      </c>
+      <c r="ARJ2">
+        <v>0.56937700000000002</v>
+      </c>
+      <c r="ARK2">
+        <v>1.3144880000000001</v>
+      </c>
+      <c r="ARL2">
+        <v>-0.208981</v>
+      </c>
+      <c r="ARM2">
+        <v>-0.135072</v>
+      </c>
+      <c r="ARN2">
+        <v>0.39676600000000001</v>
+      </c>
+      <c r="ARO2">
+        <v>1.610082</v>
+      </c>
+      <c r="ARP2">
+        <v>-1.4764170000000001</v>
+      </c>
+      <c r="ARQ2">
+        <v>1.138927</v>
+      </c>
+      <c r="ARR2">
+        <v>-0.32564799999999999</v>
+      </c>
+      <c r="ARS2">
+        <v>-0.51122299999999998</v>
+      </c>
+      <c r="ART2">
+        <v>0.16237099999999999</v>
+      </c>
+      <c r="ARU2">
+        <v>-0.75783</v>
+      </c>
+      <c r="ARV2">
+        <v>0.70237099999999997</v>
+      </c>
+      <c r="ARW2">
+        <v>-0.210006</v>
+      </c>
+      <c r="ARX2">
+        <v>-1.4541930000000001</v>
+      </c>
+      <c r="ARY2">
+        <v>0.52390999999999999</v>
+      </c>
+      <c r="ARZ2">
+        <v>-0.462173</v>
+      </c>
+      <c r="ASA2">
+        <v>-0.335314</v>
+      </c>
+      <c r="ASB2">
+        <v>-1.325359</v>
+      </c>
+      <c r="ASC2">
+        <v>1.0011110000000001</v>
+      </c>
+      <c r="ASD2">
+        <v>-0.83285500000000001</v>
+      </c>
+      <c r="ASE2">
+        <v>1.8722920000000001</v>
+      </c>
+      <c r="ASF2">
+        <v>-1.126987</v>
+      </c>
+      <c r="ASG2">
+        <v>-1.861218</v>
+      </c>
+      <c r="ASH2">
+        <v>-1.7164330000000001</v>
+      </c>
+      <c r="ASI2">
+        <v>-0.72248299999999999</v>
+      </c>
+      <c r="ASJ2">
+        <v>0.37039499999999997</v>
+      </c>
+      <c r="ASK2">
+        <v>0.30852200000000002</v>
+      </c>
+      <c r="ASL2">
+        <v>0.68382900000000002</v>
+      </c>
+      <c r="ASM2">
+        <v>-0.84190500000000001</v>
+      </c>
+      <c r="ASN2">
+        <v>-0.48502000000000001</v>
+      </c>
+      <c r="ASO2">
+        <v>-0.18889400000000001</v>
+      </c>
+      <c r="ASP2">
+        <v>1.125421</v>
+      </c>
+      <c r="ASQ2">
+        <v>-0.85317699999999996</v>
+      </c>
+      <c r="ASR2">
+        <v>-0.84200399999999997</v>
+      </c>
+      <c r="ASS2">
+        <v>-0.51318900000000001</v>
+      </c>
+      <c r="AST2">
+        <v>0.244619</v>
+      </c>
+      <c r="ASU2">
+        <v>1.358481</v>
+      </c>
+      <c r="ASV2">
+        <v>-1.5212460000000001</v>
+      </c>
+      <c r="ASW2">
+        <v>-0.77142999999999995</v>
+      </c>
+      <c r="ASX2">
+        <v>0.15120600000000001</v>
+      </c>
+      <c r="ASY2">
+        <v>0.39555499999999999</v>
+      </c>
+      <c r="ASZ2">
+        <v>0.76354</v>
+      </c>
+      <c r="ATA2">
+        <v>-0.38440800000000003</v>
+      </c>
+      <c r="ATB2">
+        <v>0.67103100000000004</v>
+      </c>
+      <c r="ATC2">
+        <v>0.26726100000000003</v>
+      </c>
+      <c r="ATD2">
+        <v>0.57175600000000004</v>
+      </c>
+      <c r="ATE2">
+        <v>0.22726299999999999</v>
+      </c>
+      <c r="ATF2">
+        <v>0.91019700000000003</v>
+      </c>
+      <c r="ATG2">
+        <v>0.30177500000000002</v>
+      </c>
+      <c r="ATH2">
+        <v>-0.50885199999999997</v>
+      </c>
+      <c r="ATI2">
+        <v>-0.19364799999999999</v>
+      </c>
+      <c r="ATJ2">
+        <v>-0.609738</v>
+      </c>
+      <c r="ATK2">
+        <v>1.537309</v>
+      </c>
+      <c r="ATL2">
+        <v>0.34572900000000001</v>
+      </c>
+      <c r="ATM2">
+        <v>1.442726</v>
+      </c>
+      <c r="ATN2">
+        <v>-3.3660000000000002E-2</v>
+      </c>
+      <c r="ATO2">
+        <v>-2.3584809999999998</v>
+      </c>
+      <c r="ATP2">
+        <v>1.8082370000000001</v>
+      </c>
+      <c r="ATQ2">
+        <v>3.5831000000000002E-2</v>
+      </c>
+      <c r="ATR2">
+        <v>1.980726</v>
+      </c>
+      <c r="ATS2">
+        <v>0.64542200000000005</v>
+      </c>
+      <c r="ATT2">
+        <v>3.8946000000000001E-2</v>
+      </c>
+      <c r="ATU2">
+        <v>1.6483509999999999</v>
+      </c>
+      <c r="ATV2">
+        <v>2.3285689999999999</v>
+      </c>
+      <c r="ATW2">
+        <v>-0.15425900000000001</v>
+      </c>
+      <c r="ATX2">
+        <v>0.16738800000000001</v>
+      </c>
+      <c r="ATY2">
+        <v>-0.52923900000000001</v>
+      </c>
+      <c r="ATZ2">
+        <v>0.52077799999999996</v>
+      </c>
+      <c r="AUA2">
+        <v>1.4606239999999999</v>
+      </c>
+      <c r="AUB2">
+        <v>-0.30571500000000001</v>
+      </c>
+      <c r="AUC2">
+        <v>-7.7066999999999997E-2</v>
+      </c>
+      <c r="AUD2">
+        <v>0.25795200000000001</v>
+      </c>
+      <c r="AUE2">
+        <v>1.814446</v>
+      </c>
+      <c r="AUF2">
+        <v>0.36108299999999999</v>
+      </c>
+      <c r="AUG2">
+        <v>0.49993399999999999</v>
+      </c>
+      <c r="AUH2">
+        <v>-0.23182</v>
+      </c>
+      <c r="AUI2">
+        <v>0.54918199999999995</v>
+      </c>
+      <c r="AUJ2">
+        <v>0.66532000000000002</v>
+      </c>
+      <c r="AUK2">
+        <v>0.78603299999999998</v>
+      </c>
+      <c r="AUL2">
+        <v>0.50112800000000002</v>
+      </c>
+      <c r="AUM2">
+        <v>-1.8557159999999999</v>
+      </c>
+      <c r="AUN2">
+        <v>0.34265400000000001</v>
+      </c>
+      <c r="AUO2">
+        <v>0.42594300000000002</v>
+      </c>
+      <c r="AUP2">
+        <v>0.15135599999999999</v>
+      </c>
+      <c r="AUQ2">
+        <v>-2.0685959999999999</v>
+      </c>
+      <c r="AUR2">
+        <v>0.41745500000000002</v>
+      </c>
+      <c r="AUS2">
+        <v>1.508286</v>
+      </c>
+      <c r="AUT2">
+        <v>0.72822100000000001</v>
+      </c>
+      <c r="AUU2">
+        <v>0.23339399999999999</v>
+      </c>
+      <c r="AUV2">
+        <v>0.91588199999999997</v>
+      </c>
+      <c r="AUW2">
+        <v>-1.3375E-2</v>
+      </c>
+      <c r="AUX2">
+        <v>3.2668000000000003E-2</v>
+      </c>
+      <c r="AUY2">
+        <v>1.436572</v>
+      </c>
+      <c r="AUZ2">
+        <v>8.8176000000000004E-2</v>
+      </c>
+      <c r="AVA2">
+        <v>-0.416184</v>
+      </c>
+      <c r="AVB2">
+        <v>1.519061</v>
+      </c>
+      <c r="AVC2">
+        <v>-2.1774269999999998</v>
+      </c>
+      <c r="AVD2">
+        <v>0.56656899999999999</v>
+      </c>
+      <c r="AVE2">
+        <v>-0.97111599999999998</v>
+      </c>
+      <c r="AVF2">
+        <v>-1.1487799999999999</v>
+      </c>
+      <c r="AVG2">
+        <v>0.14050599999999999</v>
+      </c>
+      <c r="AVH2">
+        <v>0.72267099999999995</v>
+      </c>
+      <c r="AVI2">
+        <v>-3.1336000000000003E-2</v>
+      </c>
+      <c r="AVJ2">
+        <v>1.495644</v>
+      </c>
+      <c r="AVK2">
+        <v>-0.76854699999999998</v>
+      </c>
+      <c r="AVL2">
+        <v>-0.53420500000000004</v>
+      </c>
+      <c r="AVM2">
+        <v>0.299427</v>
+      </c>
+      <c r="AVN2">
+        <v>1.4273960000000001</v>
+      </c>
+      <c r="AVO2">
+        <v>1.5925849999999999</v>
+      </c>
+      <c r="AVP2">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="AVQ2">
+        <v>-1.0513170000000001</v>
+      </c>
+      <c r="AVR2">
+        <v>-0.831179</v>
+      </c>
+      <c r="AVS2">
+        <v>4.8057000000000002E-2</v>
+      </c>
+      <c r="AVT2">
+        <v>-0.83823899999999996</v>
+      </c>
+      <c r="AVU2">
+        <v>0.48991400000000002</v>
+      </c>
+      <c r="AVV2">
+        <v>-1.095496</v>
+      </c>
+      <c r="AVW2">
+        <v>0.26303300000000002</v>
+      </c>
+      <c r="AVX2">
+        <v>0.71075900000000003</v>
+      </c>
+      <c r="AVY2">
+        <v>0.95446600000000004</v>
+      </c>
+      <c r="AVZ2">
+        <v>-0.14341999999999999</v>
+      </c>
+      <c r="AWA2">
+        <v>-0.347916</v>
+      </c>
+      <c r="AWB2">
+        <v>-0.44461800000000001</v>
+      </c>
+      <c r="AWC2">
+        <v>-5.8129999999999996E-3</v>
+      </c>
+      <c r="AWD2">
+        <v>0.82165100000000002</v>
+      </c>
+      <c r="AWE2">
+        <v>-0.17738999999999999</v>
+      </c>
+      <c r="AWF2">
+        <v>0.89537199999999995</v>
+      </c>
+      <c r="AWG2">
+        <v>-1.561115</v>
+      </c>
+      <c r="AWH2">
+        <v>7.8918000000000002E-2</v>
+      </c>
+      <c r="AWI2">
+        <v>0.48729099999999997</v>
+      </c>
+      <c r="AWJ2">
+        <v>-0.263708</v>
+      </c>
+      <c r="AWK2">
+        <v>3.8104640000000001</v>
+      </c>
+      <c r="AWL2">
+        <v>0.27056400000000003</v>
+      </c>
+      <c r="AWM2">
+        <v>-0.12720899999999999</v>
+      </c>
+      <c r="AWN2">
+        <v>-0.48584500000000003</v>
+      </c>
+      <c r="AWO2">
+        <v>9.2405000000000001E-2</v>
+      </c>
+      <c r="AWP2">
+        <v>-0.34930499999999998</v>
+      </c>
+      <c r="AWQ2">
+        <v>-8.0725000000000005E-2</v>
+      </c>
+      <c r="AWR2">
+        <v>-0.28059099999999998</v>
+      </c>
+      <c r="AWS2">
+        <v>-2.5403999999999999E-2</v>
+      </c>
+      <c r="AWT2">
+        <v>-0.13344600000000001</v>
+      </c>
+      <c r="AWU2">
+        <v>0.30104300000000001</v>
+      </c>
+      <c r="AWV2">
+        <v>-5.2080000000000001E-2</v>
+      </c>
+      <c r="AWW2">
+        <v>-0.99283399999999999</v>
+      </c>
+      <c r="AWX2">
+        <v>1.1852259999999999</v>
+      </c>
+      <c r="AWY2">
+        <v>-0.236097</v>
+      </c>
+      <c r="AWZ2">
+        <v>0.43245400000000001</v>
+      </c>
+      <c r="AXA2">
+        <v>-0.13233400000000001</v>
+      </c>
+      <c r="AXB2">
+        <v>-4.9884999999999999E-2</v>
+      </c>
+      <c r="AXC2">
+        <v>-0.199353</v>
+      </c>
+      <c r="AXD2">
+        <v>-0.219911</v>
+      </c>
+      <c r="AXE2">
+        <v>-0.82991199999999998</v>
+      </c>
+      <c r="AXF2">
+        <v>1.491047</v>
+      </c>
+      <c r="AXG2">
+        <v>0.827878</v>
+      </c>
+      <c r="AXH2">
+        <v>-1.3431709999999999</v>
+      </c>
+      <c r="AXI2">
+        <v>-1.4150940000000001</v>
+      </c>
+      <c r="AXJ2">
+        <v>0.56775799999999998</v>
+      </c>
+      <c r="AXK2">
+        <v>9.6152000000000001E-2</v>
+      </c>
+      <c r="AXL2">
+        <v>-0.25221500000000002</v>
+      </c>
+      <c r="AXM2">
+        <v>1.0688629999999999</v>
+      </c>
+      <c r="AXN2">
+        <v>0.30638900000000002</v>
+      </c>
+      <c r="AXO2">
+        <v>1.7890870000000001</v>
+      </c>
+      <c r="AXP2">
+        <v>-0.168298</v>
+      </c>
+      <c r="AXQ2">
+        <v>-0.217807</v>
+      </c>
+      <c r="AXR2">
+        <v>5.3370000000000001E-2</v>
+      </c>
+      <c r="AXS2">
+        <v>-1.1713089999999999</v>
+      </c>
+      <c r="AXT2">
+        <v>-1.4704999999999999E-2</v>
+      </c>
+      <c r="AXU2">
+        <v>1.6625319999999999</v>
+      </c>
+      <c r="AXV2">
+        <v>-0.68633599999999995</v>
+      </c>
+      <c r="AXW2">
+        <v>7.5997999999999996E-2</v>
+      </c>
+      <c r="AXX2">
+        <v>2.9921920000000002</v>
+      </c>
+      <c r="AXY2">
+        <v>-0.77637599999999996</v>
+      </c>
+      <c r="AXZ2">
+        <v>0.486425</v>
+      </c>
+      <c r="AYA2">
+        <v>-1.3221860000000001</v>
+      </c>
+      <c r="AYB2">
+        <v>0.42874600000000002</v>
+      </c>
+      <c r="AYC2">
+        <v>0.29537000000000002</v>
+      </c>
+      <c r="AYD2">
+        <v>-3.590811</v>
+      </c>
+      <c r="AYE2">
+        <v>1.7172719999999999</v>
+      </c>
+      <c r="AYF2">
+        <v>-1.9755240000000001</v>
+      </c>
+      <c r="AYG2">
+        <v>0.75849699999999998</v>
+      </c>
+      <c r="AYH2">
+        <v>0.71321999999999997</v>
+      </c>
+      <c r="AYI2">
+        <v>-0.52250200000000002</v>
+      </c>
+      <c r="AYJ2">
+        <v>0.13384099999999999</v>
+      </c>
+      <c r="AYK2">
+        <v>-0.76607800000000004</v>
+      </c>
+      <c r="AYL2">
+        <v>-1.3214939999999999</v>
+      </c>
+      <c r="AYM2">
+        <v>-1.6566449999999999</v>
+      </c>
+      <c r="AYN2">
+        <v>-1.1342570000000001</v>
+      </c>
+      <c r="AYO2">
+        <v>-2.0718540000000001</v>
+      </c>
+      <c r="AYP2">
+        <v>-1.429937</v>
+      </c>
+      <c r="AYQ2">
+        <v>1.505336</v>
+      </c>
+      <c r="AYR2">
+        <v>-1.540869</v>
+      </c>
+      <c r="AYS2">
+        <v>-0.72332300000000005</v>
+      </c>
+      <c r="AYT2">
+        <v>-0.76499799999999996</v>
+      </c>
+      <c r="AYU2">
+        <v>0.14710500000000001</v>
+      </c>
+      <c r="AYV2">
+        <v>0.65164200000000005</v>
+      </c>
+      <c r="AYW2">
+        <v>-1.791269</v>
+      </c>
+      <c r="AYX2">
+        <v>-0.58789899999999995</v>
+      </c>
+      <c r="AYY2">
+        <v>1.2332590000000001</v>
+      </c>
+      <c r="AYZ2">
+        <v>0.83248699999999998</v>
+      </c>
+      <c r="AZA2">
+        <v>1.329852</v>
+      </c>
+      <c r="AZB2">
+        <v>-1.3787430000000001</v>
+      </c>
+      <c r="AZC2">
+        <v>0.56575799999999998</v>
+      </c>
+      <c r="AZD2">
+        <v>-2.2425760000000001</v>
+      </c>
+      <c r="AZE2">
+        <v>-1.060727</v>
+      </c>
+      <c r="AZF2">
+        <v>-0.43919799999999998</v>
+      </c>
+      <c r="AZG2">
+        <v>0.47665000000000002</v>
+      </c>
+      <c r="AZH2">
+        <v>-0.17491100000000001</v>
+      </c>
+      <c r="AZI2">
+        <v>1.1382479999999999</v>
+      </c>
+      <c r="AZJ2">
+        <v>0.25345800000000002</v>
+      </c>
+      <c r="AZK2">
+        <v>-1.5394639999999999</v>
+      </c>
+      <c r="AZL2">
+        <v>-0.63558400000000004</v>
+      </c>
+      <c r="AZM2">
+        <v>3.5272999999999999E-2</v>
+      </c>
+      <c r="AZN2">
+        <v>0.37969000000000003</v>
+      </c>
+      <c r="AZO2">
+        <v>-0.47946699999999998</v>
+      </c>
+      <c r="AZP2">
+        <v>2.1717379999999999</v>
+      </c>
+      <c r="AZQ2">
+        <v>-1.039307</v>
+      </c>
+      <c r="AZR2">
+        <v>0.90861099999999995</v>
+      </c>
+      <c r="AZS2">
+        <v>-1.6328069999999999</v>
+      </c>
+      <c r="AZT2">
+        <v>-0.98987400000000003</v>
+      </c>
+      <c r="AZU2">
+        <v>0.166209</v>
+      </c>
+      <c r="AZV2">
+        <v>1.326077</v>
+      </c>
+      <c r="AZW2">
+        <v>1.314684</v>
+      </c>
+      <c r="AZX2">
+        <v>0.99509400000000003</v>
+      </c>
+      <c r="AZY2">
+        <v>1.6384669999999999</v>
+      </c>
+      <c r="AZZ2">
+        <v>-0.487398</v>
+      </c>
+      <c r="BAA2">
+        <v>-1.0548519999999999</v>
+      </c>
+      <c r="BAB2">
+        <v>-0.61905500000000002</v>
+      </c>
+      <c r="BAC2">
+        <v>1.353437</v>
+      </c>
+      <c r="BAD2">
+        <v>0.58393099999999998</v>
+      </c>
+      <c r="BAE2">
+        <v>0.75689600000000001</v>
+      </c>
+      <c r="BAF2">
+        <v>1.346495</v>
+      </c>
+      <c r="BAG2">
+        <v>-1.2963169999999999</v>
+      </c>
+      <c r="BAH2">
+        <v>-2.2475879999999999</v>
+      </c>
+      <c r="BAI2">
+        <v>-0.90382399999999996</v>
+      </c>
+      <c r="BAJ2">
+        <v>1.6744429999999999</v>
+      </c>
+      <c r="BAK2">
+        <v>-0.59276899999999999</v>
+      </c>
+      <c r="BAL2">
+        <v>1.7258530000000001</v>
+      </c>
+      <c r="BAM2">
+        <v>-1.1377330000000001</v>
+      </c>
+      <c r="BAN2">
+        <v>-0.61821999999999999</v>
+      </c>
+      <c r="BAO2">
+        <v>-0.80896900000000005</v>
+      </c>
+      <c r="BAP2">
+        <v>-0.17737700000000001</v>
+      </c>
+      <c r="BAQ2">
+        <v>-4.0833000000000001E-2</v>
+      </c>
+      <c r="BAR2">
+        <v>-0.32120700000000002</v>
+      </c>
+      <c r="BAS2">
+        <v>-0.64266199999999996</v>
+      </c>
+      <c r="BAT2">
+        <v>0.92899200000000004</v>
+      </c>
+      <c r="BAU2">
+        <v>-1.0738749999999999</v>
+      </c>
+      <c r="BAV2">
+        <v>1.0981909999999999</v>
+      </c>
+      <c r="BAW2">
+        <v>-0.44763500000000001</v>
+      </c>
+      <c r="BAX2">
+        <v>0.30381799999999998</v>
+      </c>
+      <c r="BAY2">
+        <v>-0.307643</v>
+      </c>
+      <c r="BAZ2">
+        <v>1.39733</v>
+      </c>
+      <c r="BBA2">
+        <v>-0.86873900000000004</v>
+      </c>
+      <c r="BBB2">
+        <v>-2.3773520000000001</v>
+      </c>
+      <c r="BBC2">
+        <v>0.220031</v>
+      </c>
+      <c r="BBD2">
+        <v>-0.38475700000000002</v>
+      </c>
+      <c r="BBE2">
+        <v>-0.76071900000000003</v>
+      </c>
+      <c r="BBF2">
+        <v>-0.21854999999999999</v>
+      </c>
+      <c r="BBG2">
+        <v>0.31137100000000001</v>
+      </c>
+      <c r="BBH2">
+        <v>0.19479199999999999</v>
+      </c>
+      <c r="BBI2">
+        <v>0.89586200000000005</v>
+      </c>
+      <c r="BBJ2">
+        <v>0.431952</v>
+      </c>
+      <c r="BBK2">
+        <v>0.434757</v>
+      </c>
+      <c r="BBL2">
+        <v>0.18798400000000001</v>
+      </c>
+      <c r="BBM2">
+        <v>-0.36835899999999999</v>
+      </c>
+      <c r="BBN2">
+        <v>2.8159879999999999</v>
+      </c>
+      <c r="BBO2">
+        <v>2.1058E-2</v>
+      </c>
+      <c r="BBP2">
+        <v>1.845475</v>
+      </c>
+      <c r="BBQ2">
+        <v>0.44418800000000003</v>
+      </c>
+      <c r="BBR2">
+        <v>-1.0500430000000001</v>
+      </c>
+      <c r="BBS2">
+        <v>-1.03376</v>
+      </c>
+      <c r="BBT2">
+        <v>-1.6785890000000001</v>
+      </c>
+      <c r="BBU2">
+        <v>0.21790399999999999</v>
+      </c>
+      <c r="BBV2">
+        <v>0.123284</v>
+      </c>
+      <c r="BBW2">
+        <v>-0.60063800000000001</v>
+      </c>
+      <c r="BBX2">
+        <v>1.60423</v>
+      </c>
+      <c r="BBY2">
+        <v>1.0133970000000001</v>
+      </c>
+      <c r="BBZ2">
+        <v>0.78431300000000004</v>
+      </c>
+      <c r="BCA2">
+        <v>2.130096</v>
+      </c>
+      <c r="BCB2">
+        <v>-0.152112</v>
+      </c>
+      <c r="BCC2">
+        <v>1.648156</v>
+      </c>
+      <c r="BCD2">
+        <v>-3.2211999999999998E-2</v>
+      </c>
+      <c r="BCE2">
+        <v>0.19070599999999999</v>
+      </c>
+      <c r="BCF2">
+        <v>-0.51912100000000005</v>
+      </c>
+      <c r="BCG2">
+        <v>-2.8631E-2</v>
+      </c>
+      <c r="BCH2">
+        <v>2.112851</v>
+      </c>
+      <c r="BCI2">
+        <v>1.705327</v>
+      </c>
+      <c r="BCJ2">
+        <v>1.4727209999999999</v>
+      </c>
+      <c r="BCK2">
+        <v>2.2367620000000001</v>
+      </c>
+      <c r="BCL2">
+        <v>0.52294499999999999</v>
+      </c>
+      <c r="BCM2">
+        <v>-7.0904999999999996E-2</v>
+      </c>
+      <c r="BCN2">
+        <v>0.26016899999999998</v>
+      </c>
+      <c r="BCO2">
+        <v>1.6006800000000001</v>
+      </c>
+      <c r="BCP2">
+        <v>-0.23147100000000001</v>
+      </c>
+      <c r="BCQ2">
+        <v>2.0032960000000002</v>
+      </c>
+      <c r="BCR2">
+        <v>-0.20513000000000001</v>
+      </c>
+      <c r="BCS2">
+        <v>-1.8037179999999999</v>
+      </c>
+      <c r="BCT2">
+        <v>-0.308724</v>
+      </c>
+      <c r="BCU2">
+        <v>1.050969</v>
+      </c>
+      <c r="BCV2">
+        <v>8.2914000000000002E-2</v>
+      </c>
+      <c r="BCW2">
+        <v>0.866981</v>
+      </c>
+      <c r="BCX2">
+        <v>-1.495827</v>
+      </c>
+      <c r="BCY2">
+        <v>-1.6045879999999999</v>
+      </c>
+      <c r="BCZ2">
+        <v>-0.28452699999999997</v>
+      </c>
+      <c r="BDA2">
+        <v>0.94562199999999996</v>
+      </c>
+      <c r="BDB2">
+        <v>1.5866210000000001</v>
+      </c>
+      <c r="BDC2">
+        <v>1.8256129999999999</v>
+      </c>
+      <c r="BDD2">
+        <v>-0.30095699999999997</v>
+      </c>
+      <c r="BDE2">
+        <v>1.750715</v>
+      </c>
+      <c r="BDF2">
+        <v>0.39397399999999999</v>
+      </c>
+      <c r="BDG2">
+        <v>-2.2381519999999999</v>
+      </c>
+      <c r="BDH2">
+        <v>0.840028</v>
+      </c>
+      <c r="BDI2">
+        <v>0.61646699999999999</v>
+      </c>
+      <c r="BDJ2">
+        <v>1.310573</v>
+      </c>
+      <c r="BDK2">
+        <v>-0.41568699999999997</v>
+      </c>
+      <c r="BDL2">
+        <v>-2.0175299999999998</v>
+      </c>
+      <c r="BDM2">
+        <v>0.16545399999999999</v>
+      </c>
+      <c r="BDN2">
+        <v>-0.236792</v>
+      </c>
+      <c r="BDO2">
+        <v>-6.1004000000000003E-2</v>
+      </c>
+      <c r="BDP2">
+        <v>1.7450479999999999</v>
+      </c>
+      <c r="BDQ2">
+        <v>0.65473000000000003</v>
+      </c>
+      <c r="BDR2">
+        <v>0.46981899999999999</v>
+      </c>
+      <c r="BDS2">
+        <v>0.83955299999999999</v>
+      </c>
+      <c r="BDT2">
+        <v>-1.0535270000000001</v>
+      </c>
+      <c r="BDU2">
+        <v>-0.24742800000000001</v>
+      </c>
+      <c r="BDV2">
+        <v>0.18207499999999999</v>
+      </c>
+      <c r="BDW2">
+        <v>2.1344370000000001</v>
+      </c>
+      <c r="BDX2">
+        <v>0.39321299999999998</v>
+      </c>
+      <c r="BDY2">
+        <v>-1.090857</v>
+      </c>
+      <c r="BDZ2">
+        <v>0.41400799999999999</v>
+      </c>
+      <c r="BEA2">
+        <v>0.76632199999999995</v>
+      </c>
+      <c r="BEB2">
+        <v>2.0379999999999999E-2</v>
+      </c>
+      <c r="BEC2">
+        <v>-1.6516569999999999</v>
+      </c>
+      <c r="BED2">
+        <v>0.17622199999999999</v>
+      </c>
+      <c r="BEE2">
+        <v>1.669605</v>
+      </c>
+      <c r="BEF2">
+        <v>1.696706</v>
+      </c>
+      <c r="BEG2">
+        <v>1.7722640000000001</v>
+      </c>
+      <c r="BEH2">
+        <v>-0.45842899999999998</v>
+      </c>
+      <c r="BEI2">
+        <v>1.1115E-2</v>
+      </c>
+      <c r="BEJ2">
+        <v>-0.53909099999999999</v>
+      </c>
+      <c r="BEK2">
+        <v>0.51056900000000005</v>
+      </c>
+      <c r="BEL2">
+        <v>-1.238556</v>
+      </c>
+      <c r="BEM2">
+        <v>-0.83027099999999998</v>
+      </c>
+      <c r="BEN2">
+        <v>5.6264000000000002E-2</v>
+      </c>
+      <c r="BEO2">
+        <v>-0.65871299999999999</v>
+      </c>
+      <c r="BEP2">
+        <v>-1.4038280000000001</v>
+      </c>
+      <c r="BEQ2">
+        <v>-1.110527</v>
+      </c>
+      <c r="BER2">
+        <v>-0.51980199999999999</v>
+      </c>
+      <c r="BES2">
+        <v>-1.5913539999999999</v>
+      </c>
+      <c r="BET2">
+        <v>-0.60995900000000003</v>
+      </c>
+      <c r="BEU2">
+        <v>-0.63863599999999998</v>
+      </c>
+      <c r="BEV2">
+        <v>0.22292000000000001</v>
+      </c>
+      <c r="BEW2">
+        <v>0.588198</v>
+      </c>
+      <c r="BEX2">
+        <v>-1.678706</v>
+      </c>
+      <c r="BEY2">
+        <v>0.105906</v>
+      </c>
+      <c r="BEZ2">
+        <v>1.452116</v>
+      </c>
+      <c r="BFA2">
+        <v>-0.13858999999999999</v>
+      </c>
+      <c r="BFB2">
+        <v>0.59955499999999995</v>
+      </c>
+      <c r="BFC2">
+        <v>2.7202419999999998</v>
+      </c>
+      <c r="BFD2">
+        <v>-0.79400099999999996</v>
+      </c>
+      <c r="BFE2">
+        <v>-1.103205</v>
+      </c>
+      <c r="BFF2">
+        <v>1.8468800000000001</v>
+      </c>
+      <c r="BFG2">
+        <v>-0.84509100000000004</v>
+      </c>
+      <c r="BFH2">
+        <v>-0.12623400000000001</v>
+      </c>
+      <c r="BFI2">
+        <v>1.159351</v>
+      </c>
+      <c r="BFJ2">
+        <v>0.86119199999999996</v>
+      </c>
+      <c r="BFK2">
+        <v>0.40895599999999999</v>
+      </c>
+      <c r="BFL2">
+        <v>-0.83291400000000004</v>
+      </c>
+      <c r="BFM2">
+        <v>0.221305</v>
+      </c>
+      <c r="BFN2">
+        <v>-1.310797</v>
+      </c>
+      <c r="BFO2">
+        <v>-0.45508199999999999</v>
+      </c>
+      <c r="BFP2">
+        <v>-1.304953</v>
+      </c>
+      <c r="BFQ2">
+        <v>6.8041000000000004E-2</v>
+      </c>
+      <c r="BFR2">
+        <v>0.92049000000000003</v>
+      </c>
+      <c r="BFS2">
+        <v>1.8585879999999999</v>
+      </c>
+      <c r="BFT2">
+        <v>-0.60512600000000005</v>
+      </c>
+      <c r="BFU2">
+        <v>-0.34387600000000001</v>
+      </c>
+      <c r="BFV2">
+        <v>0.17235700000000001</v>
+      </c>
+      <c r="BFW2">
+        <v>1.3266089999999999</v>
+      </c>
+      <c r="BFX2">
+        <v>-1.3096000000000001</v>
+      </c>
+      <c r="BFY2">
+        <v>-1.0114510000000001</v>
+      </c>
+      <c r="BFZ2">
+        <v>0.92495300000000003</v>
+      </c>
+      <c r="BGA2">
+        <v>-0.17516300000000001</v>
+      </c>
+      <c r="BGB2">
+        <v>0.28731000000000001</v>
+      </c>
+      <c r="BGC2">
+        <v>-2.2090719999999999</v>
+      </c>
+      <c r="BGD2">
+        <v>-0.74221000000000004</v>
+      </c>
+      <c r="BGE2">
+        <v>0.72086099999999997</v>
+      </c>
+      <c r="BGF2">
+        <v>0.211309</v>
+      </c>
+      <c r="BGG2">
+        <v>0.70918300000000001</v>
+      </c>
+      <c r="BGH2">
+        <v>0.21420900000000001</v>
+      </c>
+      <c r="BGI2">
+        <v>-0.52705400000000002</v>
+      </c>
+      <c r="BGJ2">
+        <v>-0.55703899999999995</v>
+      </c>
+      <c r="BGK2">
+        <v>-1.276756</v>
+      </c>
+      <c r="BGL2">
+        <v>-1.737652</v>
+      </c>
+      <c r="BGM2">
+        <v>-8.4588999999999998E-2</v>
+      </c>
+      <c r="BGN2">
+        <v>-1.699622</v>
+      </c>
+      <c r="BGO2">
+        <v>-4.8598000000000002E-2</v>
+      </c>
+      <c r="BGP2">
+        <v>-1.0211859999999999</v>
+      </c>
+      <c r="BGQ2">
+        <v>2.5354040000000002</v>
+      </c>
+      <c r="BGR2">
+        <v>0.85391799999999995</v>
+      </c>
+      <c r="BGS2">
+        <v>0.46857500000000002</v>
+      </c>
+      <c r="BGT2">
+        <v>0.64493999999999996</v>
+      </c>
+      <c r="BGU2">
+        <v>1.0043120000000001</v>
+      </c>
+      <c r="BGV2">
+        <v>7.1043999999999996E-2</v>
+      </c>
+      <c r="BGW2">
+        <v>-0.57686400000000004</v>
+      </c>
+      <c r="BGX2">
+        <v>-1.28017</v>
+      </c>
+      <c r="BGY2">
+        <v>-0.27390799999999998</v>
+      </c>
+      <c r="BGZ2">
+        <v>0.17416799999999999</v>
+      </c>
+      <c r="BHA2">
+        <v>0.64221499999999998</v>
+      </c>
+      <c r="BHB2">
+        <v>0.880803</v>
+      </c>
+      <c r="BHC2">
+        <v>0.53643600000000002</v>
+      </c>
+      <c r="BHD2">
+        <v>-0.38836999999999999</v>
+      </c>
+      <c r="BHE2">
+        <v>0.78813500000000003</v>
+      </c>
+      <c r="BHF2">
+        <v>-0.74657600000000002</v>
+      </c>
+      <c r="BHG2">
+        <v>-2.004982</v>
+      </c>
+      <c r="BHH2">
+        <v>-0.60309999999999997</v>
+      </c>
+      <c r="BHI2">
+        <v>-0.47331200000000001</v>
+      </c>
+      <c r="BHJ2">
+        <v>2.8596E-2</v>
+      </c>
+      <c r="BHK2">
+        <v>-1.076999</v>
+      </c>
+      <c r="BHL2">
+        <v>6.3479999999999995E-2</v>
+      </c>
+      <c r="BHM2">
+        <v>-0.107126</v>
+      </c>
+      <c r="BHN2">
+        <v>1.4963580000000001</v>
+      </c>
+      <c r="BHO2">
+        <v>0.30743399999999999</v>
+      </c>
+      <c r="BHP2">
+        <v>-0.56437800000000005</v>
+      </c>
+      <c r="BHQ2">
+        <v>1.242372</v>
+      </c>
+      <c r="BHR2">
+        <v>-0.246785</v>
+      </c>
+      <c r="BHS2">
+        <v>0.77549199999999996</v>
+      </c>
+      <c r="BHT2">
+        <v>-0.26196000000000003</v>
+      </c>
+      <c r="BHU2">
+        <v>0.31572699999999998</v>
+      </c>
+      <c r="BHV2">
+        <v>0.53388100000000005</v>
+      </c>
+      <c r="BHW2">
+        <v>-1.8292679999999999</v>
+      </c>
+      <c r="BHX2">
+        <v>-0.29372500000000001</v>
+      </c>
+      <c r="BHY2">
+        <v>0.63485400000000003</v>
+      </c>
+      <c r="BHZ2">
+        <v>1.11208</v>
+      </c>
+      <c r="BIA2">
+        <v>-1.5502149999999999</v>
+      </c>
+      <c r="BIB2">
+        <v>-1.9199999999999998E-2</v>
+      </c>
+      <c r="BIC2">
+        <v>0.54977399999999998</v>
+      </c>
+      <c r="BID2">
+        <v>-1.477565</v>
+      </c>
+      <c r="BIE2">
+        <v>-1.695038</v>
+      </c>
+      <c r="BIF2">
+        <v>-0.57296899999999995</v>
+      </c>
+      <c r="BIG2">
+        <v>0.51726399999999995</v>
+      </c>
+      <c r="BIH2">
+        <v>0.70729900000000001</v>
+      </c>
+      <c r="BII2">
+        <v>-0.492871</v>
+      </c>
+      <c r="BIJ2">
+        <v>0.293545</v>
+      </c>
+      <c r="BIK2">
+        <v>-0.19169700000000001</v>
+      </c>
+      <c r="BIL2">
+        <v>0.42697400000000002</v>
+      </c>
+      <c r="BIM2">
+        <v>1.2973999999999999E-2</v>
+      </c>
+      <c r="BIN2">
+        <v>-0.40346300000000002</v>
+      </c>
+      <c r="BIO2">
+        <v>-0.67213400000000001</v>
+      </c>
+      <c r="BIP2">
+        <v>1.2353940000000001</v>
+      </c>
+      <c r="BIQ2">
+        <v>0.427952</v>
+      </c>
+      <c r="BIR2">
+        <v>-0.65691500000000003</v>
+      </c>
+      <c r="BIS2">
+        <v>-2.0093779999999999</v>
+      </c>
+      <c r="BIT2">
+        <v>-0.85484700000000002</v>
+      </c>
+      <c r="BIU2">
+        <v>2.182687</v>
+      </c>
+      <c r="BIV2">
+        <v>-0.54420199999999996</v>
+      </c>
+      <c r="BIW2">
+        <v>1.2425470000000001</v>
+      </c>
+      <c r="BIX2">
+        <v>-0.67832599999999998</v>
+      </c>
+      <c r="BIY2">
+        <v>0.89410199999999995</v>
+      </c>
+      <c r="BIZ2">
+        <v>-0.97677199999999997</v>
+      </c>
+      <c r="BJA2">
+        <v>1.151376</v>
+      </c>
+      <c r="BJB2">
+        <v>0.72380800000000001</v>
+      </c>
+      <c r="BJC2">
+        <v>-0.76785199999999998</v>
+      </c>
+      <c r="BJD2">
+        <v>-0.52399600000000002</v>
+      </c>
+      <c r="BJE2">
+        <v>0.223384</v>
+      </c>
+      <c r="BJF2">
+        <v>0.565419</v>
+      </c>
+      <c r="BJG2">
+        <v>-2.097836</v>
+      </c>
+      <c r="BJH2">
+        <v>0.24907099999999999</v>
+      </c>
+      <c r="BJI2">
+        <v>-4.4082999999999997E-2</v>
+      </c>
+      <c r="BJJ2">
+        <v>1.092479</v>
+      </c>
+      <c r="BJK2">
+        <v>-0.558778</v>
+      </c>
+      <c r="BJL2">
+        <v>1.087764</v>
+      </c>
+      <c r="BJM2">
+        <v>0.43626799999999999</v>
+      </c>
+      <c r="BJN2">
+        <v>1.1297509999999999</v>
+      </c>
+      <c r="BJO2">
+        <v>1.389276</v>
+      </c>
+      <c r="BJP2">
+        <v>-0.263156</v>
+      </c>
+      <c r="BJQ2">
+        <v>0.21005399999999999</v>
+      </c>
+      <c r="BJR2">
+        <v>-0.41068700000000002</v>
+      </c>
+      <c r="BJS2">
+        <v>-0.68541399999999997</v>
+      </c>
+      <c r="BJT2">
+        <v>-0.17377799999999999</v>
+      </c>
+      <c r="BJU2">
+        <v>0.178975</v>
+      </c>
+      <c r="BJV2">
+        <v>-1.152852</v>
+      </c>
+      <c r="BJW2">
+        <v>0.806392</v>
+      </c>
+      <c r="BJX2">
+        <v>-0.69707399999999997</v>
+      </c>
+      <c r="BJY2">
+        <v>0.32795200000000002</v>
+      </c>
+      <c r="BJZ2">
+        <v>-0.97647600000000001</v>
+      </c>
+      <c r="BKA2">
+        <v>0.78683899999999996</v>
+      </c>
+      <c r="BKB2">
+        <v>0.78027800000000003</v>
+      </c>
+      <c r="BKC2">
+        <v>1.5589459999999999</v>
+      </c>
+      <c r="BKD2">
+        <v>-1.7846880000000001</v>
+      </c>
+      <c r="BKE2">
+        <v>-2.334794</v>
+      </c>
+      <c r="BKF2">
+        <v>1.4616290000000001</v>
+      </c>
+      <c r="BKG2">
+        <v>0.65217099999999995</v>
+      </c>
+      <c r="BKH2">
+        <v>0.42821900000000002</v>
+      </c>
+      <c r="BKI2">
+        <v>-0.75852799999999998</v>
+      </c>
+      <c r="BKJ2">
+        <v>0.48561399999999999</v>
+      </c>
+      <c r="BKK2">
+        <v>5.3768000000000003E-2</v>
+      </c>
+      <c r="BKL2">
+        <v>-1.4992080000000001</v>
+      </c>
+      <c r="BKM2">
+        <v>1.7886070000000001</v>
+      </c>
+      <c r="BKN2">
+        <v>0.91572500000000001</v>
+      </c>
+      <c r="BKO2">
+        <v>0.157717</v>
+      </c>
+      <c r="BKP2">
+        <v>-9.0658000000000002E-2</v>
+      </c>
+      <c r="BKQ2">
+        <v>0.24399699999999999</v>
+      </c>
+      <c r="BKR2">
+        <v>0.27258900000000003</v>
+      </c>
+      <c r="BKS2">
+        <v>0.57451799999999997</v>
+      </c>
+      <c r="BKT2">
+        <v>0.46196799999999999</v>
+      </c>
+      <c r="BKU2">
+        <v>1.046041</v>
+      </c>
+      <c r="BKV2">
+        <v>0.38567400000000002</v>
+      </c>
+      <c r="BKW2">
+        <v>-1.5419579999999999</v>
+      </c>
+      <c r="BKX2">
+        <v>0.80629499999999998</v>
+      </c>
+      <c r="BKY2">
+        <v>1.243144</v>
+      </c>
+      <c r="BKZ2">
+        <v>0.83821699999999999</v>
+      </c>
+      <c r="BLA2">
+        <v>2.135205</v>
+      </c>
+      <c r="BLB2">
+        <v>-0.119101</v>
+      </c>
+      <c r="BLC2">
+        <v>-3.6908999999999997E-2</v>
+      </c>
+      <c r="BLD2">
+        <v>1.9201490000000001</v>
+      </c>
+      <c r="BLE2">
+        <v>-0.92478000000000005</v>
+      </c>
+      <c r="BLF2">
+        <v>-0.42370799999999997</v>
+      </c>
+      <c r="BLG2">
+        <v>-0.68631600000000004</v>
+      </c>
+      <c r="BLH2">
+        <v>1.1032930000000001</v>
+      </c>
+      <c r="BLI2">
+        <v>-0.36492799999999997</v>
+      </c>
+      <c r="BLJ2">
+        <v>0.46684599999999998</v>
+      </c>
+      <c r="BLK2">
+        <v>0.28037899999999999</v>
+      </c>
+      <c r="BLL2">
+        <v>-0.17050499999999999</v>
+      </c>
+      <c r="BLM2">
+        <v>1.414342</v>
+      </c>
+      <c r="BLN2">
+        <v>-1.1716880000000001</v>
+      </c>
+      <c r="BLO2">
+        <v>0.24585899999999999</v>
+      </c>
+      <c r="BLP2">
+        <v>0.95180500000000001</v>
+      </c>
+      <c r="BLQ2">
+        <v>1.2215659999999999</v>
+      </c>
+      <c r="BLR2">
+        <v>1.36694</v>
+      </c>
+      <c r="BLS2">
+        <v>-0.11863</v>
+      </c>
+      <c r="BLT2">
+        <v>-1.2092510000000001</v>
+      </c>
+      <c r="BLU2">
+        <v>0.87938099999999997</v>
+      </c>
+      <c r="BLV2">
+        <v>0.63297999999999999</v>
+      </c>
+      <c r="BLW2">
+        <v>-6.2601000000000004E-2</v>
+      </c>
+      <c r="BLX2">
+        <v>-0.12884599999999999</v>
+      </c>
+      <c r="BLY2">
+        <v>0.49034899999999998</v>
+      </c>
+      <c r="BLZ2">
+        <v>1.5627470000000001</v>
+      </c>
+      <c r="BMA2">
+        <v>0.42392099999999999</v>
+      </c>
+      <c r="BMB2">
+        <v>0.81011500000000003</v>
+      </c>
+      <c r="BMC2">
+        <v>0.72927600000000004</v>
+      </c>
+      <c r="BMD2">
+        <v>1.188482</v>
+      </c>
+      <c r="BME2">
+        <v>1.388245</v>
+      </c>
+      <c r="BMF2">
+        <v>-0.49161300000000002</v>
+      </c>
+      <c r="BMG2">
+        <v>1.792986</v>
+      </c>
+      <c r="BMH2">
+        <v>0.88624700000000001</v>
+      </c>
+      <c r="BMI2">
+        <v>0.93318199999999996</v>
+      </c>
+      <c r="BMJ2">
+        <v>1.3563860000000001</v>
+      </c>
+      <c r="BMK2">
+        <v>0.386795</v>
+      </c>
+      <c r="BML2">
+        <v>-0.366734</v>
+      </c>
+      <c r="BMM2">
+        <v>0.84911599999999998</v>
+      </c>
+      <c r="BMN2">
+        <v>0.51089799999999996</v>
+      </c>
+      <c r="BMO2">
+        <v>0.46004</v>
+      </c>
+      <c r="BMP2">
+        <v>-8.4779999999999994E-2</v>
+      </c>
+      <c r="BMQ2">
+        <v>-0.93013699999999999</v>
+      </c>
+      <c r="BMR2">
+        <v>-1.6715500000000001</v>
+      </c>
+      <c r="BMS2">
+        <v>-0.19454399999999999</v>
+      </c>
+      <c r="BMT2">
+        <v>0.33463799999999999</v>
+      </c>
+      <c r="BMU2">
+        <v>-0.24237900000000001</v>
+      </c>
+      <c r="BMV2">
+        <v>0.49685800000000002</v>
+      </c>
+      <c r="BMW2">
+        <v>-1.3062039999999999</v>
+      </c>
+      <c r="BMX2">
+        <v>-0.12662300000000001</v>
+      </c>
+      <c r="BMY2">
+        <v>-0.283578</v>
+      </c>
+      <c r="BMZ2">
+        <v>0.40842099999999998</v>
+      </c>
+      <c r="BNA2">
+        <v>-0.73667700000000003</v>
+      </c>
+      <c r="BNB2">
+        <v>0.15288399999999999</v>
+      </c>
+      <c r="BNC2">
+        <v>-0.96555199999999997</v>
+      </c>
+      <c r="BND2">
+        <v>0.26738800000000001</v>
+      </c>
+      <c r="BNE2">
+        <v>-0.30382500000000001</v>
+      </c>
+      <c r="BNF2">
+        <v>0.98674399999999995</v>
+      </c>
+      <c r="BNG2">
+        <v>-0.231651</v>
+      </c>
+      <c r="BNH2">
+        <v>0.59176499999999999</v>
+      </c>
+      <c r="BNI2">
+        <v>1.3103469999999999</v>
+      </c>
+      <c r="BNJ2">
+        <v>0.91492099999999998</v>
+      </c>
+      <c r="BNK2">
+        <v>1.086705</v>
+      </c>
+      <c r="BNL2">
+        <v>-1.814279</v>
+      </c>
+      <c r="BNM2">
+        <v>0.85963400000000001</v>
+      </c>
+      <c r="BNN2">
+        <v>0.88011099999999998</v>
+      </c>
+      <c r="BNO2">
+        <v>1.5440419999999999</v>
+      </c>
+      <c r="BNP2">
+        <v>-2.5101490000000002</v>
+      </c>
+      <c r="BNQ2">
+        <v>-2.9100999999999998E-2</v>
+      </c>
+      <c r="BNR2">
+        <v>-0.14704600000000001</v>
+      </c>
+      <c r="BNS2">
+        <v>1.2473380000000001</v>
+      </c>
+      <c r="BNT2">
+        <v>1.0477529999999999</v>
+      </c>
+      <c r="BNU2">
+        <v>0.67951499999999998</v>
+      </c>
+      <c r="BNV2">
+        <v>1.4968220000000001</v>
+      </c>
+      <c r="BNW2">
+        <v>3.7124999999999998E-2</v>
+      </c>
+      <c r="BNX2">
+        <v>1.3563529999999999</v>
+      </c>
+      <c r="BNY2">
+        <v>-0.55662500000000004</v>
+      </c>
+      <c r="BNZ2">
+        <v>1.633084</v>
+      </c>
+      <c r="BOA2">
+        <v>3.4761E-2</v>
+      </c>
+      <c r="BOB2">
+        <v>-0.30042999999999997</v>
+      </c>
+      <c r="BOC2">
+        <v>1.853947</v>
+      </c>
+      <c r="BOD2">
+        <v>-0.77712999999999999</v>
+      </c>
+      <c r="BOE2">
+        <v>0.80665900000000001</v>
+      </c>
+      <c r="BOF2">
+        <v>0.394397</v>
+      </c>
+      <c r="BOG2">
+        <v>3.702E-3</v>
+      </c>
+      <c r="BOH2">
+        <v>-0.14061599999999999</v>
+      </c>
+      <c r="BOI2">
+        <v>-0.99197199999999996</v>
+      </c>
+      <c r="BOJ2">
+        <v>1.1016490000000001</v>
+      </c>
+      <c r="BOK2">
+        <v>-1.010567</v>
+      </c>
+      <c r="BOL2">
+        <v>-5.2832999999999998E-2</v>
+      </c>
+      <c r="BOM2">
+        <v>-1.5188219999999999</v>
+      </c>
+      <c r="BON2">
+        <v>1.3803099999999999</v>
+      </c>
+      <c r="BOO2">
+        <v>-1.9058280000000001</v>
+      </c>
+      <c r="BOP2">
+        <v>1.0225770000000001</v>
+      </c>
+      <c r="BOQ2">
+        <v>0.15017900000000001</v>
+      </c>
+      <c r="BOR2">
+        <v>1.967827</v>
+      </c>
+      <c r="BOS2">
+        <v>-0.17216799999999999</v>
+      </c>
+      <c r="BOT2">
+        <v>1.577734</v>
+      </c>
+      <c r="BOU2">
+        <v>0.51254699999999997</v>
+      </c>
+      <c r="BOV2">
+        <v>-0.37293399999999999</v>
+      </c>
+      <c r="BOW2">
+        <v>1.1587350000000001</v>
+      </c>
+      <c r="BOX2">
+        <v>9.7575999999999996E-2</v>
+      </c>
+      <c r="BOY2">
+        <v>0.82519600000000004</v>
+      </c>
+      <c r="BOZ2">
+        <v>-0.121082</v>
+      </c>
+      <c r="BPA2">
+        <v>0.91388199999999997</v>
+      </c>
+      <c r="BPB2">
+        <v>0.681091</v>
+      </c>
+      <c r="BPC2">
+        <v>0.86209400000000003</v>
+      </c>
+      <c r="BPD2">
+        <v>-0.30123699999999998</v>
+      </c>
+      <c r="BPE2">
+        <v>1.205643</v>
+      </c>
+      <c r="BPF2">
+        <v>-0.48721300000000001</v>
+      </c>
+      <c r="BPG2">
+        <v>-0.57163200000000003</v>
+      </c>
+      <c r="BPH2">
+        <v>-1.064694</v>
+      </c>
+      <c r="BPI2">
+        <v>-0.423064</v>
+      </c>
+      <c r="BPJ2">
+        <v>-0.67620899999999995</v>
+      </c>
+      <c r="BPK2">
+        <v>-0.73325300000000004</v>
+      </c>
+      <c r="BPL2">
+        <v>0.28921999999999998</v>
+      </c>
+      <c r="BPM2">
+        <v>-0.94062299999999999</v>
+      </c>
+      <c r="BPN2">
+        <v>-0.13330800000000001</v>
+      </c>
+      <c r="BPO2">
+        <v>0.58746900000000002</v>
+      </c>
+      <c r="BPP2">
+        <v>0.98434900000000003</v>
+      </c>
+      <c r="BPQ2">
+        <v>0.243752</v>
+      </c>
+      <c r="BPR2">
+        <v>-0.48835299999999998</v>
+      </c>
+      <c r="BPS2">
+        <v>0.57745899999999994</v>
+      </c>
+      <c r="BPT2">
+        <v>-2.0967159999999998</v>
+      </c>
+      <c r="BPU2">
+        <v>-0.64251800000000003</v>
+      </c>
+      <c r="BPV2">
+        <v>-0.53242100000000003</v>
+      </c>
+      <c r="BPW2">
+        <v>1.3319859999999999</v>
+      </c>
+      <c r="BPX2">
+        <v>1.6833</v>
+      </c>
+      <c r="BPY2">
+        <v>0.42077799999999999</v>
+      </c>
+      <c r="BPZ2">
+        <v>-1.24583</v>
+      </c>
+      <c r="BQA2">
+        <v>0.34797</v>
+      </c>
+      <c r="BQB2">
+        <v>0.94219900000000001</v>
+      </c>
+      <c r="BQC2">
+        <v>-0.78155699999999995</v>
+      </c>
+      <c r="BQD2">
+        <v>1.087431</v>
+      </c>
+      <c r="BQE2">
+        <v>1.0932120000000001</v>
+      </c>
+      <c r="BQF2">
+        <v>-0.97145999999999999</v>
+      </c>
+      <c r="BQG2">
+        <v>2.3433440000000001</v>
+      </c>
+      <c r="BQH2">
+        <v>0.53656499999999996</v>
+      </c>
+      <c r="BQI2">
+        <v>0.51674699999999996</v>
+      </c>
+      <c r="BQJ2">
+        <v>-0.74785400000000002</v>
+      </c>
+      <c r="BQK2">
+        <v>-1.2029510000000001</v>
+      </c>
+      <c r="BQL2">
+        <v>-1.248912</v>
+      </c>
+      <c r="BQM2">
+        <v>-0.73651599999999995</v>
+      </c>
+      <c r="BQN2">
+        <v>-0.25335400000000002</v>
+      </c>
+      <c r="BQO2">
+        <v>1.2985089999999999</v>
+      </c>
+      <c r="BQP2">
+        <v>-0.66022400000000003</v>
+      </c>
+      <c r="BQQ2">
+        <v>-1.1399319999999999</v>
+      </c>
+      <c r="BQR2">
+        <v>1.07236</v>
+      </c>
+      <c r="BQS2">
+        <v>0.141293</v>
+      </c>
+      <c r="BQT2">
+        <v>-1.6152219999999999</v>
+      </c>
+      <c r="BQU2">
+        <v>-8.6292999999999995E-2</v>
+      </c>
+      <c r="BQV2">
+        <v>0.328372</v>
+      </c>
+      <c r="BQW2">
+        <v>-1.5107790000000001</v>
+      </c>
+      <c r="BQX2">
+        <v>0.27984100000000001</v>
+      </c>
+      <c r="BQY2">
+        <v>-1.2400180000000001</v>
+      </c>
+      <c r="BQZ2">
+        <v>0.64717199999999997</v>
+      </c>
+      <c r="BRA2">
+        <v>2.5820439999999998</v>
+      </c>
+      <c r="BRB2">
+        <v>-0.85480599999999995</v>
+      </c>
+      <c r="BRC2">
+        <v>0.20386199999999999</v>
+      </c>
+      <c r="BRD2">
+        <v>-0.44033699999999998</v>
+      </c>
+      <c r="BRE2">
+        <v>-0.789655</v>
+      </c>
+      <c r="BRF2">
+        <v>-0.98526100000000005</v>
+      </c>
+      <c r="BRG2">
+        <v>-1.4192450000000001</v>
+      </c>
+      <c r="BRH2">
+        <v>0.89882899999999999</v>
+      </c>
+      <c r="BRI2">
+        <v>0.18972900000000001</v>
+      </c>
+      <c r="BRJ2">
+        <v>-0.19966100000000001</v>
+      </c>
+      <c r="BRK2">
+        <v>1.6101049999999999</v>
+      </c>
+      <c r="BRL2">
+        <v>-1.311903</v>
+      </c>
+      <c r="BRM2">
+        <v>0.89893199999999995</v>
+      </c>
+      <c r="BRN2">
+        <v>0.95748200000000006</v>
+      </c>
+      <c r="BRO2">
+        <v>0.15076500000000001</v>
+      </c>
+      <c r="BRP2">
+        <v>-2.7481450000000001</v>
+      </c>
+      <c r="BRQ2">
+        <v>-1.8491390000000001</v>
+      </c>
+      <c r="BRR2">
+        <v>-1.7681530000000001</v>
+      </c>
+      <c r="BRS2">
+        <v>0.61296399999999995</v>
+      </c>
+      <c r="BRT2">
+        <v>0.20142599999999999</v>
+      </c>
+      <c r="BRU2">
+        <v>0.73774300000000004</v>
+      </c>
+      <c r="BRV2">
+        <v>0.15104500000000001</v>
+      </c>
+      <c r="BRW2">
+        <v>-0.82074199999999997</v>
+      </c>
+      <c r="BRX2">
+        <v>0.14482300000000001</v>
+      </c>
+      <c r="BRY2">
+        <v>0.29314200000000001</v>
+      </c>
+      <c r="BRZ2">
+        <v>-0.28074700000000002</v>
+      </c>
+      <c r="BSA2">
+        <v>-1.2545999999999999</v>
+      </c>
+      <c r="BSB2">
+        <v>0.93093800000000004</v>
+      </c>
+      <c r="BSC2">
+        <v>0.72750000000000004</v>
+      </c>
+      <c r="BSD2">
+        <v>1.307256</v>
+      </c>
+      <c r="BSE2">
+        <v>0.90371999999999997</v>
+      </c>
+      <c r="BSF2">
+        <v>-0.841449</v>
+      </c>
+      <c r="BSG2">
+        <v>0.60612299999999997</v>
+      </c>
+      <c r="BSH2">
+        <v>-0.32128299999999999</v>
+      </c>
+      <c r="BSI2">
+        <v>0.24804200000000001</v>
+      </c>
+      <c r="BSJ2">
+        <v>-0.33105099999999998</v>
+      </c>
+      <c r="BSK2">
+        <v>-0.24823899999999999</v>
+      </c>
+      <c r="BSL2">
+        <v>-0.64193</v>
+      </c>
+      <c r="BSM2">
+        <v>-0.13453499999999999</v>
+      </c>
+      <c r="BSN2">
+        <v>0.37969599999999998</v>
+      </c>
+      <c r="BSO2">
+        <v>-0.75339900000000004</v>
+      </c>
+      <c r="BSP2">
+        <v>0.94603499999999996</v>
+      </c>
+      <c r="BSQ2">
+        <v>0.32905499999999999</v>
+      </c>
+      <c r="BSR2">
+        <v>-0.44677699999999998</v>
+      </c>
+      <c r="BSS2">
+        <v>1.8378369999999999</v>
+      </c>
+      <c r="BST2">
+        <v>-0.887957</v>
+      </c>
+      <c r="BSU2">
+        <v>-1.271941</v>
+      </c>
+      <c r="BSV2">
+        <v>1.8343560000000001</v>
+      </c>
+      <c r="BSW2">
+        <v>1.6575500000000001</v>
+      </c>
+      <c r="BSX2">
+        <v>0.43607400000000002</v>
+      </c>
+      <c r="BSY2">
+        <v>0.47658800000000001</v>
+      </c>
+      <c r="BSZ2">
+        <v>0.24818499999999999</v>
+      </c>
+      <c r="BTA2">
+        <v>-1.0492589999999999</v>
+      </c>
+      <c r="BTB2">
+        <v>0.102591</v>
+      </c>
+      <c r="BTC2">
+        <v>-0.63110200000000005</v>
+      </c>
+      <c r="BTD2">
+        <v>0.55074000000000001</v>
+      </c>
+      <c r="BTE2">
+        <v>5.4198999999999997E-2</v>
+      </c>
+      <c r="BTF2">
+        <v>-0.983039</v>
+      </c>
+      <c r="BTG2">
+        <v>0.63735900000000001</v>
+      </c>
+      <c r="BTH2">
+        <v>1.7487360000000001</v>
+      </c>
+      <c r="BTI2">
+        <v>6.1889E-2</v>
+      </c>
+      <c r="BTJ2">
+        <v>0.55686999999999998</v>
+      </c>
+      <c r="BTK2">
+        <v>-1.6381479999999999</v>
+      </c>
+      <c r="BTL2">
+        <v>-2.5298389999999999</v>
+      </c>
+      <c r="BTM2">
+        <v>-0.88072600000000001</v>
+      </c>
+      <c r="BTN2">
+        <v>-0.65611399999999998</v>
+      </c>
+      <c r="BTO2">
+        <v>-1.2334080000000001</v>
+      </c>
+      <c r="BTP2">
+        <v>-0.55624799999999996</v>
+      </c>
+      <c r="BTQ2">
+        <v>-2.9309000000000002E-2</v>
+      </c>
+      <c r="BTR2">
+        <v>-0.22386</v>
+      </c>
+      <c r="BTS2">
+        <v>-0.50613900000000001</v>
+      </c>
+      <c r="BTT2">
+        <v>0.33579399999999998</v>
+      </c>
+      <c r="BTU2">
+        <v>1.9507239999999999</v>
+      </c>
+      <c r="BTV2">
+        <v>0.70519100000000001</v>
+      </c>
+      <c r="BTW2">
+        <v>-4.5189E-2</v>
+      </c>
+      <c r="BTX2">
+        <v>0.37145800000000001</v>
+      </c>
+      <c r="BTY2">
+        <v>-0.53139999999999998</v>
+      </c>
+      <c r="BTZ2">
+        <v>1.7470600000000001</v>
+      </c>
+      <c r="BUA2">
+        <v>0.47600500000000001</v>
+      </c>
+      <c r="BUB2">
+        <v>-1.0423720000000001</v>
+      </c>
+      <c r="BUC2">
+        <v>1.1949110000000001</v>
+      </c>
+      <c r="BUD2">
+        <v>0.18779699999999999</v>
+      </c>
+      <c r="BUE2">
+        <v>0.941137</v>
+      </c>
+      <c r="BUF2">
+        <v>-0.89386500000000002</v>
+      </c>
+      <c r="BUG2">
+        <v>-0.70545400000000003</v>
+      </c>
+      <c r="BUH2">
+        <v>0.81343900000000002</v>
+      </c>
+      <c r="BUI2">
+        <v>0.67766800000000005</v>
+      </c>
+      <c r="BUJ2">
+        <v>5.8096000000000002E-2</v>
+      </c>
+      <c r="BUK2">
+        <v>3.4091999999999997E-2</v>
+      </c>
+      <c r="BUL2">
+        <v>0.59446100000000002</v>
+      </c>
+      <c r="BUM2">
+        <v>-0.33765299999999998</v>
+      </c>
+      <c r="BUN2">
+        <v>-0.77856400000000003</v>
+      </c>
+      <c r="BUO2">
+        <v>-5.2727000000000003E-2</v>
+      </c>
+      <c r="BUP2">
+        <v>-0.66435900000000003</v>
+      </c>
+      <c r="BUQ2">
+        <v>9.7567000000000001E-2</v>
+      </c>
+      <c r="BUR2">
+        <v>-0.15801999999999999</v>
+      </c>
+      <c r="BUS2">
+        <v>0.24234600000000001</v>
+      </c>
+      <c r="BUT2">
+        <v>-2.3772060000000002</v>
+      </c>
+      <c r="BUU2">
+        <v>-0.62558400000000003</v>
+      </c>
+      <c r="BUV2">
+        <v>-2.1741809999999999</v>
+      </c>
+      <c r="BUW2">
+        <v>-0.15140999999999999</v>
+      </c>
+      <c r="BUX2">
+        <v>-0.64176299999999997</v>
+      </c>
+      <c r="BUY2">
+        <v>1.2209669999999999</v>
+      </c>
+      <c r="BUZ2">
+        <v>-1.180283</v>
+      </c>
+      <c r="BVA2">
+        <v>1.572403</v>
+      </c>
+      <c r="BVB2">
+        <v>0.570882</v>
+      </c>
+      <c r="BVC2">
+        <v>1.1674990000000001</v>
+      </c>
+      <c r="BVD2">
+        <v>-0.23527999999999999</v>
+      </c>
+      <c r="BVE2">
+        <v>0.40253499999999998</v>
+      </c>
+      <c r="BVF2">
+        <v>-0.25506200000000001</v>
+      </c>
+      <c r="BVG2">
+        <v>0.35696499999999998</v>
+      </c>
+      <c r="BVH2">
+        <v>4.8311E-2</v>
+      </c>
+      <c r="BVI2">
+        <v>0.37311100000000003</v>
+      </c>
+      <c r="BVJ2">
+        <v>-1.1316759999999999</v>
+      </c>
+      <c r="BVK2">
+        <v>-0.49135299999999998</v>
+      </c>
+      <c r="BVL2">
+        <v>-1.1639759999999999</v>
+      </c>
+      <c r="BVM2">
+        <v>-0.88570800000000005</v>
+      </c>
+      <c r="BVN2">
+        <v>2.1915300000000002</v>
+      </c>
+      <c r="BVO2">
+        <v>-0.99728000000000006</v>
+      </c>
+      <c r="BVP2">
+        <v>0.643316</v>
+      </c>
+      <c r="BVQ2">
+        <v>0.44941500000000001</v>
+      </c>
+      <c r="BVR2">
+        <v>2.532969</v>
+      </c>
+      <c r="BVS2">
+        <v>0.13511300000000001</v>
+      </c>
+      <c r="BVT2">
+        <v>-1.436375</v>
+      </c>
+      <c r="BVU2">
+        <v>-8.2439999999999999E-2</v>
+      </c>
+      <c r="BVV2">
+        <v>1.6640790000000001</v>
+      </c>
+      <c r="BVW2">
+        <v>1.1806890000000001</v>
+      </c>
+      <c r="BVX2">
+        <v>0.65490400000000004</v>
+      </c>
+      <c r="BVY2">
+        <v>0.54652900000000004</v>
+      </c>
+      <c r="BVZ2">
+        <v>0.491066</v>
+      </c>
+      <c r="BWA2">
+        <v>1.697811</v>
+      </c>
+      <c r="BWB2">
+        <v>0.61039600000000005</v>
+      </c>
+      <c r="BWC2">
+        <v>-1.194801</v>
+      </c>
+      <c r="BWD2">
+        <v>0.340472</v>
+      </c>
+      <c r="BWE2">
+        <v>-0.139684</v>
+      </c>
+      <c r="BWF2">
+        <v>-0.39818900000000002</v>
+      </c>
+      <c r="BWG2">
+        <v>1.5704979999999999</v>
+      </c>
+      <c r="BWH2">
+        <v>0.97827299999999995</v>
+      </c>
+      <c r="BWI2">
+        <v>0.48315200000000003</v>
+      </c>
+      <c r="BWJ2">
+        <v>-0.34274300000000002</v>
+      </c>
+      <c r="BWK2">
+        <v>-0.42736800000000003</v>
+      </c>
+      <c r="BWL2">
+        <v>-0.99633000000000005</v>
+      </c>
+      <c r="BWM2">
+        <v>0.15525800000000001</v>
+      </c>
+      <c r="BWN2">
+        <v>-0.58158500000000002</v>
+      </c>
+      <c r="BWO2">
+        <v>-1.130457</v>
+      </c>
+      <c r="BWP2">
+        <v>-0.250585</v>
+      </c>
+      <c r="BWQ2">
+        <v>1.576047</v>
+      </c>
+      <c r="BWR2">
+        <v>9.5856999999999998E-2</v>
+      </c>
+      <c r="BWS2">
+        <v>1.1405149999999999</v>
+      </c>
+      <c r="BWT2">
+        <v>-0.59661900000000001</v>
+      </c>
+      <c r="BWU2">
+        <v>6.1366999999999998E-2</v>
+      </c>
+      <c r="BWV2">
+        <v>2.0212999999999998E-2</v>
+      </c>
+      <c r="BWW2">
+        <v>-0.80343200000000004</v>
+      </c>
+      <c r="BWX2">
+        <v>-0.54872600000000005</v>
+      </c>
+      <c r="BWY2">
+        <v>-1.3788400000000001</v>
+      </c>
+      <c r="BWZ2">
+        <v>-1.8940129999999999</v>
+      </c>
+      <c r="BXA2">
+        <v>-0.18266299999999999</v>
+      </c>
+      <c r="BXB2">
+        <v>6.0204000000000001E-2</v>
+      </c>
+      <c r="BXC2">
+        <v>-0.27055200000000001</v>
+      </c>
+      <c r="BXD2">
+        <v>1.840625</v>
+      </c>
+      <c r="BXE2">
+        <v>-0.34442600000000001</v>
+      </c>
+      <c r="BXF2">
+        <v>0.70865</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1982" x14ac:dyDescent="0.35">
+      <c r="AKS6">
+        <f>COLUMN(AKU3)</f>
+        <v>983</v>
+      </c>
+      <c r="BXB6">
+        <f>COLUMN(BXF3)</f>
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1982" x14ac:dyDescent="0.35">
+      <c r="ALJ9">
+        <f>COLUMN(ALL3)</f>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>